<commit_message>
Atualizando dados da planilha de hipóteses
</commit_message>
<xml_diff>
--- a/HIPOTESES.xlsx
+++ b/HIPOTESES.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\ProjetosPython\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0A58D0-F19A-4565-9847-063F358EA223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A04AAC-269E-4E6F-BEDB-F3E29BA33716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DFE4666F-66AA-47B4-B4D1-4475D501A3D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$F$840</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4092" uniqueCount="2129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4140" uniqueCount="2176">
   <si>
     <t>TIPO</t>
   </si>
@@ -6435,13 +6438,154 @@
   </si>
   <si>
     <t>TENDINITE NO TORNOZELO ESQUERDO E DIRETO</t>
+  </si>
+  <si>
+    <t>RMCOTOVDIR</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, cotovelo, direito</t>
+  </si>
+  <si>
+    <t>RMCOTOVESQ</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, cotovelo, esquerdo</t>
+  </si>
+  <si>
+    <t>RMJOELHODIR</t>
+  </si>
+  <si>
+    <t>RMJOELHOESQ</t>
+  </si>
+  <si>
+    <t>RMMAODIR</t>
+  </si>
+  <si>
+    <t>RMMAOESQ</t>
+  </si>
+  <si>
+    <t>RMOMBRODIR</t>
+  </si>
+  <si>
+    <t>RMOMBROESQ</t>
+  </si>
+  <si>
+    <t>RMPERNADIR</t>
+  </si>
+  <si>
+    <t>RMPERNAESQ</t>
+  </si>
+  <si>
+    <t>RMPUNHODIR</t>
+  </si>
+  <si>
+    <t>RMPUNHOESQ</t>
+  </si>
+  <si>
+    <t>RMQUADRILDIR</t>
+  </si>
+  <si>
+    <t>RMQUADRILESQ</t>
+  </si>
+  <si>
+    <t>RMTORNODIR</t>
+  </si>
+  <si>
+    <t>RMTORNOESQ</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, joelho, direito</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, joelho, esquerdo</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, mão, direita</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, mão, esquerda</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, ombro, direito</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, ombro, esquerdo</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, perna, direita</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, perna, esquerda</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, punho, direito</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, punho, esquerdo</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, quadril, direito</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, quadril, esquerdo</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, tornozelo, direito</t>
+  </si>
+  <si>
+    <t>Ressonância magnética, tornozelo, esquerdo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESSONÂNCIA MAGNÉTICA DE COTOVELO DIREITO PARA AVALIAÇÃO AFECÇÕES INFLAMATÓRIAS E LESÕES MUSCULARES  </t>
+  </si>
+  <si>
+    <t>RESSONÂNCIA MAGNÉTICA DE JOELHO DIREITO PARA AVALIAÇÃO DE FRATURAS E  AFECÇÕES INFLAMATÓRIAS INFECCIOSAS</t>
+  </si>
+  <si>
+    <t>RESSONÂNCIA MAGNÉTICA DE JOELHO ESQUERDO PARA AVALIAÇÃO DE FRATURAS E  AFECÇÕES INFLAMATÓRIAS INFECCIOSAS</t>
+  </si>
+  <si>
+    <t>Avaliar em detalhe as estruturas da mão esquerda, incluindo ossos, cartilagens, ligamentos, tendões, músculos e nervos</t>
+  </si>
+  <si>
+    <t>Avaliar em detalhe as estruturas da mão direita , incluindo ossos, cartilagens, ligamentos, tendões, músculos e nervos</t>
+  </si>
+  <si>
+    <t>RESSONÂNCIA MAGNÉTICA DE OMBRO DIREITO PARA AVALIAÇÃO DE FRATURAS E TENDINITE LIGAMENTAR AGUDA</t>
+  </si>
+  <si>
+    <t>RESSONÂNCIA MAGNÉTICA DE OMBRO ESQUERDO PARA AVALIAÇÃO DE FRATURAS E TENDINITE LIGAMENTAR AGUDA</t>
+  </si>
+  <si>
+    <t>RESSONÂNCIA MAGNÉTICA DE PERNA DIREITA PARA AVALIAÇÃO DE  ESPAÇO ARTICULAR E LESÃO MUSCULAR GRAVE     </t>
+  </si>
+  <si>
+    <t>RESSONÂNCIA MAGNÉTICA DE PERNA ESQUERDA PARA AVALIAÇÃO DE  ESPAÇO ARTICULAR E LESÃO MUSCULAR GRAVE     </t>
+  </si>
+  <si>
+    <t>RESSONANCIA MAGNÉTICA DE PUNHO DIREITO PARA AVALIAÇÃO DE LESÃO/FRATURAS</t>
+  </si>
+  <si>
+    <t>RESSONANCIA MAGNÉTICA DE PUNHO ESQUERDO PARA AVALIAÇÃO DE LESÃO/FRATURAS</t>
+  </si>
+  <si>
+    <t>RESSONÂNCIA MAGNÉTICA DE QUADRIL DIREITO PARA AVALIAÇÃO DE AFECÇÕES INFLAMATÓRIAS E LESÕES DO LÁBRUM ACETABULAR</t>
+  </si>
+  <si>
+    <t>RESSONÂNCIA MAGNÉTICA DE QUADRIL ESQUERDO PARA AVALIAÇÃO DE AFECÇÕES INFLAMATÓRIAS E LESÕES DO LÁBRUM ACETABULAR</t>
+  </si>
+  <si>
+    <t>TENDINITE NO TORNOZELO DIREITO</t>
+  </si>
+  <si>
+    <t>TENDINITE NO TORNOZELO ESQUERDO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6534,6 +6678,27 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -6598,7 +6763,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -6621,6 +6786,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7297,10 +7465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F598A03-C175-48A4-8B4B-F3666B999AEE}">
-  <dimension ref="A1:F822"/>
+  <dimension ref="A1:F872"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C388" workbookViewId="0">
-      <selection activeCell="F415" sqref="F415"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22073,11 +22241,311 @@
         <v>2125</v>
       </c>
     </row>
+    <row r="823" spans="1:6">
+      <c r="A823" s="21" t="s">
+        <v>2129</v>
+      </c>
+      <c r="B823" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="F823" s="3" t="s">
+        <v>2161</v>
+      </c>
+    </row>
+    <row r="824" spans="1:6">
+      <c r="A824" s="21" t="s">
+        <v>2131</v>
+      </c>
+      <c r="B824" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="F824" s="3" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="825" spans="1:6">
+      <c r="A825" s="21" t="s">
+        <v>2133</v>
+      </c>
+      <c r="B825" s="20" t="s">
+        <v>2147</v>
+      </c>
+      <c r="F825" s="3" t="s">
+        <v>2162</v>
+      </c>
+    </row>
+    <row r="826" spans="1:6">
+      <c r="A826" s="21" t="s">
+        <v>2134</v>
+      </c>
+      <c r="B826" s="20" t="s">
+        <v>2148</v>
+      </c>
+      <c r="F826" s="3" t="s">
+        <v>2163</v>
+      </c>
+    </row>
+    <row r="827" spans="1:6">
+      <c r="A827" s="21" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B827" s="20" t="s">
+        <v>2149</v>
+      </c>
+      <c r="F827" s="3" t="s">
+        <v>2165</v>
+      </c>
+    </row>
+    <row r="828" spans="1:6">
+      <c r="A828" s="21" t="s">
+        <v>2136</v>
+      </c>
+      <c r="B828" s="20" t="s">
+        <v>2150</v>
+      </c>
+      <c r="F828" s="3" t="s">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="829" spans="1:6">
+      <c r="A829" s="21" t="s">
+        <v>2137</v>
+      </c>
+      <c r="B829" s="20" t="s">
+        <v>2151</v>
+      </c>
+      <c r="F829" s="3" t="s">
+        <v>2166</v>
+      </c>
+    </row>
+    <row r="830" spans="1:6">
+      <c r="A830" s="21" t="s">
+        <v>2138</v>
+      </c>
+      <c r="B830" s="20" t="s">
+        <v>2152</v>
+      </c>
+      <c r="F830" s="3" t="s">
+        <v>2167</v>
+      </c>
+    </row>
+    <row r="831" spans="1:6">
+      <c r="A831" s="21" t="s">
+        <v>2139</v>
+      </c>
+      <c r="B831" s="20" t="s">
+        <v>2153</v>
+      </c>
+      <c r="F831" s="3" t="s">
+        <v>2168</v>
+      </c>
+    </row>
+    <row r="832" spans="1:6">
+      <c r="A832" s="21" t="s">
+        <v>2140</v>
+      </c>
+      <c r="B832" s="20" t="s">
+        <v>2154</v>
+      </c>
+      <c r="F832" s="3" t="s">
+        <v>2169</v>
+      </c>
+    </row>
+    <row r="833" spans="1:6">
+      <c r="A833" s="21" t="s">
+        <v>2141</v>
+      </c>
+      <c r="B833" s="20" t="s">
+        <v>2155</v>
+      </c>
+      <c r="F833" s="3" t="s">
+        <v>2170</v>
+      </c>
+    </row>
+    <row r="834" spans="1:6">
+      <c r="A834" s="21" t="s">
+        <v>2142</v>
+      </c>
+      <c r="B834" s="20" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F834" s="3" t="s">
+        <v>2171</v>
+      </c>
+    </row>
+    <row r="835" spans="1:6">
+      <c r="A835" s="21" t="s">
+        <v>2143</v>
+      </c>
+      <c r="B835" s="20" t="s">
+        <v>2157</v>
+      </c>
+      <c r="F835" s="16" t="s">
+        <v>2172</v>
+      </c>
+    </row>
+    <row r="836" spans="1:6">
+      <c r="A836" s="21" t="s">
+        <v>2144</v>
+      </c>
+      <c r="B836" s="20" t="s">
+        <v>2158</v>
+      </c>
+      <c r="F836" s="16" t="s">
+        <v>2173</v>
+      </c>
+    </row>
+    <row r="837" spans="1:6">
+      <c r="A837" s="21" t="s">
+        <v>2145</v>
+      </c>
+      <c r="B837" s="20" t="s">
+        <v>2159</v>
+      </c>
+      <c r="F837" s="3" t="s">
+        <v>2174</v>
+      </c>
+    </row>
+    <row r="838" spans="1:6">
+      <c r="A838" s="21" t="s">
+        <v>2146</v>
+      </c>
+      <c r="B838" s="20" t="s">
+        <v>2160</v>
+      </c>
+      <c r="F838" s="3" t="s">
+        <v>2175</v>
+      </c>
+    </row>
+    <row r="839" spans="1:6">
+      <c r="A839" s="21"/>
+      <c r="B839" s="20"/>
+    </row>
+    <row r="840" spans="1:6">
+      <c r="A840" s="21"/>
+      <c r="B840" s="20"/>
+    </row>
+    <row r="841" spans="1:6">
+      <c r="A841" s="21"/>
+      <c r="B841" s="20"/>
+    </row>
+    <row r="842" spans="1:6">
+      <c r="A842" s="21"/>
+      <c r="B842" s="20"/>
+    </row>
+    <row r="843" spans="1:6">
+      <c r="A843" s="21"/>
+      <c r="B843" s="20"/>
+    </row>
+    <row r="844" spans="1:6">
+      <c r="A844" s="21"/>
+      <c r="B844" s="20"/>
+    </row>
+    <row r="845" spans="1:6">
+      <c r="A845" s="21"/>
+      <c r="B845" s="20"/>
+    </row>
+    <row r="846" spans="1:6">
+      <c r="A846" s="21"/>
+      <c r="B846" s="20"/>
+    </row>
+    <row r="847" spans="1:6">
+      <c r="A847" s="21"/>
+      <c r="B847" s="20"/>
+    </row>
+    <row r="848" spans="1:6">
+      <c r="A848" s="21"/>
+      <c r="B848" s="20"/>
+    </row>
+    <row r="849" spans="1:2">
+      <c r="A849" s="21"/>
+      <c r="B849" s="20"/>
+    </row>
+    <row r="850" spans="1:2">
+      <c r="A850" s="21"/>
+      <c r="B850" s="20"/>
+    </row>
+    <row r="851" spans="1:2">
+      <c r="A851" s="21"/>
+      <c r="B851" s="20"/>
+    </row>
+    <row r="852" spans="1:2">
+      <c r="A852" s="21"/>
+      <c r="B852" s="20"/>
+    </row>
+    <row r="853" spans="1:2">
+      <c r="A853" s="21"/>
+      <c r="B853" s="20"/>
+    </row>
+    <row r="854" spans="1:2">
+      <c r="A854" s="22"/>
+      <c r="B854" s="20"/>
+    </row>
+    <row r="855" spans="1:2">
+      <c r="A855" s="22"/>
+      <c r="B855" s="20"/>
+    </row>
+    <row r="856" spans="1:2">
+      <c r="A856" s="22"/>
+      <c r="B856" s="20"/>
+    </row>
+    <row r="857" spans="1:2">
+      <c r="A857" s="22"/>
+      <c r="B857" s="20"/>
+    </row>
+    <row r="858" spans="1:2">
+      <c r="A858" s="22"/>
+      <c r="B858" s="20"/>
+    </row>
+    <row r="859" spans="1:2">
+      <c r="A859" s="22"/>
+      <c r="B859" s="20"/>
+    </row>
+    <row r="860" spans="1:2">
+      <c r="A860" s="22"/>
+    </row>
+    <row r="861" spans="1:2">
+      <c r="A861" s="22"/>
+    </row>
+    <row r="862" spans="1:2">
+      <c r="A862" s="22"/>
+    </row>
+    <row r="863" spans="1:2">
+      <c r="A863" s="22"/>
+    </row>
+    <row r="864" spans="1:2">
+      <c r="A864" s="22"/>
+    </row>
+    <row r="865" spans="1:1">
+      <c r="A865" s="22"/>
+    </row>
+    <row r="866" spans="1:1">
+      <c r="A866" s="22"/>
+    </row>
+    <row r="867" spans="1:1">
+      <c r="A867" s="22"/>
+    </row>
+    <row r="868" spans="1:1">
+      <c r="A868" s="22"/>
+    </row>
+    <row r="869" spans="1:1">
+      <c r="A869" s="22"/>
+    </row>
+    <row r="870" spans="1:1">
+      <c r="A870" s="22"/>
+    </row>
+    <row r="871" spans="1:1">
+      <c r="A871" s="22"/>
+    </row>
+    <row r="872" spans="1:1">
+      <c r="A872" s="22"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 *** Este documento está classificado como INTERNO pelo GRUPO FLEURY ***</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>